<commit_message>
words v0.13 - member_word_history 테이블의 trigger 제거
. cafe24에서 trigger 미지원에 따라 trigger 대신 프로그램 로직으로 구현
</commit_message>
<xml_diff>
--- a/words/sql/문제 가중치 산정식.xlsx
+++ b/words/sql/문제 가중치 산정식.xlsx
@@ -198,7 +198,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -268,11 +268,11 @@
         <v>24</v>
       </c>
       <c r="E4" s="0" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F4" s="0" t="n">
         <f aca="false">A4*E4</f>
-        <v>52</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -302,11 +302,11 @@
         <v>40</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">A6*E6</f>
-        <v>124</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,7 +367,7 @@
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">SUM(F1:F9)</f>
-        <v>672</v>
+        <v>584</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
words v0.14 - questions_correct_by_level view를 테이블로 변경
</commit_message>
<xml_diff>
--- a/words/sql/문제 가중치 산정식.xlsx
+++ b/words/sql/문제 가중치 산정식.xlsx
@@ -29,8 +29,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="YYYY&quot;년 &quot;M&quot;월 &quot;D\일"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -109,12 +110,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -195,10 +200,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+      <selection pane="topLeft" activeCell="F15" activeCellId="0" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -301,12 +306,13 @@
         <f aca="false">B5+C$2</f>
         <v>40</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <v>0.5</v>
+      <c r="E6" s="2" t="n">
+        <f aca="false">6/19</f>
+        <v>0.31578947368421</v>
       </c>
       <c r="F6" s="0" t="n">
         <f aca="false">A6*E6</f>
-        <v>62</v>
+        <v>39.1578947368421</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -319,11 +325,11 @@
         <v>48</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F7" s="0" t="n">
         <f aca="false">A7*E7</f>
-        <v>172</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -367,7 +373,11 @@
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">SUM(F1:F9)</f>
-        <v>584</v>
+        <v>475.157894736842</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <f aca="false">(1000-F11)/10</f>
+        <v>52.4842105263158</v>
       </c>
     </row>
   </sheetData>

</xml_diff>